<commit_message>
Se agrega funcionalidad para Menú
</commit_message>
<xml_diff>
--- a/chats/50242041486@c.us.xlsx
+++ b/chats/50242041486@c.us.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>Fecha</t>
   </si>
@@ -101,6 +101,27 @@
   </si>
   <si>
     <t>22-04-2022 08:42</t>
+  </si>
+  <si>
+    <t>03-05-2022 08:39</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>03-05-2022 09:22</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>03-05-2022 09:23</t>
+  </si>
+  <si>
+    <t>03-05-2022 09:24</t>
+  </si>
+  <si>
+    <t>Adios</t>
   </si>
 </sst>
 </file>
@@ -477,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B33"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -688,6 +709,62 @@
         <v>3</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Se mejora el menú
</commit_message>
<xml_diff>
--- a/chats/50242041486@c.us.xlsx
+++ b/chats/50242041486@c.us.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>Fecha</t>
   </si>
@@ -122,6 +122,27 @@
   </si>
   <si>
     <t>Adios</t>
+  </si>
+  <si>
+    <t>03-05-2022 09:39</t>
+  </si>
+  <si>
+    <t>03-05-2022 09:42</t>
+  </si>
+  <si>
+    <t>03-05-2022 09:48</t>
+  </si>
+  <si>
+    <t>03-05-2022 09:49</t>
+  </si>
+  <si>
+    <t>03-05-2022 09:51</t>
+  </si>
+  <si>
+    <t>03-05-2022 09:52</t>
+  </si>
+  <si>
+    <t>03-05-2022 09:53</t>
   </si>
 </sst>
 </file>
@@ -498,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B46"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -765,6 +786,110 @@
         <v>36</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>